<commit_message>
Rewrote Celina's Excel into CSVs
Signed-off-by: jeenyjinjin <43344567+jeenyjinjin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Data/Course Learning Outcomes (Technical Skills) V2.xlsx
+++ b/Data/Course Learning Outcomes (Technical Skills) V2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\celinakoh\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin\Desktop\IS480 FYP\ChickenDinner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3582048D-FE36-4AA3-870F-5D9689D6984D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8295" tabRatio="634"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8295" tabRatio="634" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills &amp; Competencies" sheetId="2" r:id="rId1"/>
@@ -31,13 +32,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
     <author>Celina KOH</author>
   </authors>
   <commentList>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="1" shapeId="0">
+    <comment ref="C20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="0" shapeId="0">
+    <comment ref="I25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S32" authorId="0" shapeId="0">
+    <comment ref="S32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="0" shapeId="0">
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="1" shapeId="0">
+    <comment ref="C38" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="1" shapeId="0">
+    <comment ref="B47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -195,10 +196,10 @@
         </r>
       </text>
     </comment>
-    <comment ref="C60" authorId="1" shapeId="0">
+    <comment ref="C60" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text/>
     </comment>
-    <comment ref="K60" authorId="1" shapeId="0">
+    <comment ref="K60" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -228,12 +229,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0" shapeId="0">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -277,12 +278,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -308,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0" shapeId="0">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2672,7 +2673,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3810,165 +3811,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4042,80 +3884,239 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4410,14 +4411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4439,11 +4440,11 @@
     <col min="28" max="16384" width="8.7109375" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="177" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="178" t="s">
+    <row r="1" spans="1:29" s="124" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="125" t="s">
         <v>774</v>
       </c>
-      <c r="B1" s="176"/>
+      <c r="B1" s="123"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -4556,7 +4557,7 @@
       <c r="AC2" s="38"/>
     </row>
     <row r="3" spans="1:29" s="25" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="178" t="s">
         <v>121</v>
       </c>
       <c r="B3" s="118" t="s">
@@ -4606,7 +4607,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="130"/>
+      <c r="A4" s="179"/>
       <c r="B4" s="91" t="s">
         <v>306</v>
       </c>
@@ -4673,7 +4674,7 @@
       <c r="AC4" s="25"/>
     </row>
     <row r="5" spans="1:29" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="130"/>
+      <c r="A5" s="179"/>
       <c r="B5" s="92" t="s">
         <v>307</v>
       </c>
@@ -4703,7 +4704,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="92" t="s">
         <v>308</v>
       </c>
@@ -4757,7 +4758,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" s="25" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
+      <c r="A7" s="179"/>
       <c r="B7" s="92" t="s">
         <v>310</v>
       </c>
@@ -4808,7 +4809,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
+      <c r="A8" s="179"/>
       <c r="B8" s="92" t="s">
         <v>320</v>
       </c>
@@ -4865,7 +4866,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
+      <c r="A9" s="179"/>
       <c r="B9" s="92" t="s">
         <v>311</v>
       </c>
@@ -4916,7 +4917,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="179"/>
       <c r="B10" s="92" t="s">
         <v>312</v>
       </c>
@@ -4961,7 +4962,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
+      <c r="A11" s="179"/>
       <c r="B11" s="92" t="s">
         <v>313</v>
       </c>
@@ -5024,7 +5025,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
+      <c r="A12" s="179"/>
       <c r="B12" s="92" t="s">
         <v>305</v>
       </c>
@@ -5083,7 +5084,7 @@
       <c r="AC12" s="25"/>
     </row>
     <row r="13" spans="1:29" s="26" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="131"/>
+      <c r="A13" s="180"/>
       <c r="B13" s="120" t="s">
         <v>321</v>
       </c>
@@ -5154,7 +5155,7 @@
       <c r="AC13" s="25"/>
     </row>
     <row r="14" spans="1:29" s="76" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="132" t="s">
+      <c r="A14" s="181" t="s">
         <v>115</v>
       </c>
       <c r="B14" s="93" t="s">
@@ -5233,7 +5234,7 @@
       <c r="AC14" s="27"/>
     </row>
     <row r="15" spans="1:29" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
+      <c r="A15" s="182"/>
       <c r="B15" s="94" t="s">
         <v>246</v>
       </c>
@@ -5299,7 +5300,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
+      <c r="A16" s="182"/>
       <c r="B16" s="94" t="s">
         <v>248</v>
       </c>
@@ -5365,7 +5366,7 @@
       </c>
     </row>
     <row r="17" spans="1:29" s="81" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="133"/>
+      <c r="A17" s="182"/>
       <c r="B17" s="95" t="s">
         <v>253</v>
       </c>
@@ -5438,7 +5439,7 @@
       <c r="AC17" s="27"/>
     </row>
     <row r="18" spans="1:29" s="75" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="134"/>
+      <c r="A18" s="183"/>
       <c r="B18" s="114" t="s">
         <v>251</v>
       </c>
@@ -5493,7 +5494,7 @@
       <c r="AC18" s="74"/>
     </row>
     <row r="19" spans="1:29" s="82" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="187" t="s">
         <v>741</v>
       </c>
       <c r="B19" s="96" t="s">
@@ -5564,11 +5565,11 @@
       <c r="AC19" s="28"/>
     </row>
     <row r="20" spans="1:29" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="139"/>
+      <c r="A20" s="188"/>
       <c r="B20" s="97" t="s">
         <v>256</v>
       </c>
-      <c r="C20" s="179" t="s">
+      <c r="C20" s="126" t="s">
         <v>261</v>
       </c>
       <c r="D20" s="28" t="s">
@@ -5633,7 +5634,7 @@
       </c>
     </row>
     <row r="21" spans="1:29" s="28" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="139"/>
+      <c r="A21" s="188"/>
       <c r="B21" s="97" t="s">
         <v>422</v>
       </c>
@@ -5678,7 +5679,7 @@
       </c>
     </row>
     <row r="22" spans="1:29" s="83" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="139"/>
+      <c r="A22" s="188"/>
       <c r="B22" s="98" t="s">
         <v>258</v>
       </c>
@@ -5723,7 +5724,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="139"/>
+      <c r="A23" s="188"/>
       <c r="B23" s="98" t="s">
         <v>260</v>
       </c>
@@ -5733,29 +5734,29 @@
       <c r="D23" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="E23" s="180" t="s">
+      <c r="E23" s="127" t="s">
         <v>643</v>
       </c>
-      <c r="F23" s="180" t="s">
+      <c r="F23" s="127" t="s">
         <v>644</v>
       </c>
-      <c r="G23" s="180" t="s">
+      <c r="G23" s="127" t="s">
         <v>645</v>
       </c>
-      <c r="H23" s="180" t="s">
+      <c r="H23" s="127" t="s">
         <v>646</v>
       </c>
-      <c r="I23" s="180" t="s">
+      <c r="I23" s="127" t="s">
         <v>647</v>
       </c>
-      <c r="J23" s="180" t="s">
+      <c r="J23" s="127" t="s">
         <v>648</v>
       </c>
-      <c r="K23" s="180" t="s">
+      <c r="K23" s="127" t="s">
         <v>455</v>
       </c>
-      <c r="L23" s="180"/>
-      <c r="O23" s="181" t="s">
+      <c r="L23" s="127"/>
+      <c r="O23" s="128" t="s">
         <v>400</v>
       </c>
       <c r="P23" s="28" t="s">
@@ -5763,7 +5764,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="139"/>
+      <c r="A24" s="188"/>
       <c r="B24" s="97" t="s">
         <v>263</v>
       </c>
@@ -5823,7 +5824,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="139"/>
+      <c r="A25" s="188"/>
       <c r="B25" s="97" t="s">
         <v>265</v>
       </c>
@@ -5876,7 +5877,7 @@
       <c r="AC25" s="28"/>
     </row>
     <row r="26" spans="1:29" s="84" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="139"/>
+      <c r="A26" s="188"/>
       <c r="B26" s="99" t="s">
         <v>267</v>
       </c>
@@ -5936,9 +5937,9 @@
       <c r="AB26" s="28"/>
       <c r="AC26" s="28"/>
     </row>
-    <row r="27" spans="1:29" s="184" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="140"/>
-      <c r="B27" s="182" t="s">
+    <row r="27" spans="1:29" s="131" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="189"/>
+      <c r="B27" s="129" t="s">
         <v>632</v>
       </c>
       <c r="C27" s="28" t="s">
@@ -5947,7 +5948,7 @@
       <c r="D27" s="28" t="s">
         <v>634</v>
       </c>
-      <c r="E27" s="183" t="s">
+      <c r="E27" s="130" t="s">
         <v>677</v>
       </c>
       <c r="F27" s="28" t="s">
@@ -5992,7 +5993,7 @@
       <c r="AC27" s="28"/>
     </row>
     <row r="28" spans="1:29" s="77" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="141" t="s">
+      <c r="A28" s="190" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="100" t="s">
@@ -6055,7 +6056,7 @@
       <c r="AC28" s="32"/>
     </row>
     <row r="29" spans="1:29" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="142"/>
+      <c r="A29" s="191"/>
       <c r="B29" s="101" t="s">
         <v>271</v>
       </c>
@@ -6133,7 +6134,7 @@
       </c>
     </row>
     <row r="30" spans="1:29" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="142"/>
+      <c r="A30" s="191"/>
       <c r="B30" s="102" t="s">
         <v>273</v>
       </c>
@@ -6183,47 +6184,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="185" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="142"/>
+    <row r="31" spans="1:29" s="132" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="191"/>
       <c r="B31" s="102" t="s">
         <v>275</v>
       </c>
-      <c r="C31" s="185" t="s">
+      <c r="C31" s="132" t="s">
         <v>274</v>
       </c>
-      <c r="D31" s="185" t="s">
+      <c r="D31" s="132" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="185" t="s">
+      <c r="E31" s="132" t="s">
         <v>463</v>
       </c>
-      <c r="F31" s="185" t="s">
+      <c r="F31" s="132" t="s">
         <v>665</v>
       </c>
-      <c r="G31" s="185" t="s">
+      <c r="G31" s="132" t="s">
         <v>664</v>
       </c>
-      <c r="H31" s="185" t="s">
+      <c r="H31" s="132" t="s">
         <v>660</v>
       </c>
-      <c r="I31" s="185" t="s">
+      <c r="I31" s="132" t="s">
         <v>661</v>
       </c>
-      <c r="J31" s="185" t="s">
+      <c r="J31" s="132" t="s">
         <v>662</v>
       </c>
-      <c r="K31" s="185" t="s">
+      <c r="K31" s="132" t="s">
         <v>666</v>
       </c>
-      <c r="O31" s="185" t="s">
+      <c r="O31" s="132" t="s">
         <v>667</v>
       </c>
-      <c r="P31" s="185" t="s">
+      <c r="P31" s="132" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="186" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="142"/>
+    <row r="32" spans="1:29" s="133" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="191"/>
       <c r="B32" s="102" t="s">
         <v>277</v>
       </c>
@@ -6303,9 +6304,9 @@
       <c r="AB32" s="32"/>
       <c r="AC32" s="32"/>
     </row>
-    <row r="33" spans="1:132" s="186" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="142"/>
-      <c r="B33" s="187" t="s">
+    <row r="33" spans="1:132" s="133" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="191"/>
+      <c r="B33" s="134" t="s">
         <v>279</v>
       </c>
       <c r="C33" s="32" t="s">
@@ -6379,7 +6380,7 @@
       <c r="AC33" s="32"/>
     </row>
     <row r="34" spans="1:132" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="142"/>
+      <c r="A34" s="191"/>
       <c r="B34" s="102" t="s">
         <v>635</v>
       </c>
@@ -6418,7 +6419,7 @@
       </c>
     </row>
     <row r="35" spans="1:132" s="113" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="143"/>
+      <c r="A35" s="192"/>
       <c r="B35" s="112" t="s">
         <v>637</v>
       </c>
@@ -6455,7 +6456,7 @@
       <c r="AC35" s="111"/>
     </row>
     <row r="36" spans="1:132" s="86" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135" t="s">
+      <c r="A36" s="184" t="s">
         <v>118</v>
       </c>
       <c r="B36" s="103" t="s">
@@ -6514,7 +6515,7 @@
       <c r="AC36" s="110"/>
     </row>
     <row r="37" spans="1:132" s="87" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="136"/>
+      <c r="A37" s="185"/>
       <c r="B37" s="104" t="s">
         <v>285</v>
       </c>
@@ -6568,7 +6569,7 @@
       </c>
     </row>
     <row r="38" spans="1:132" s="116" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="136"/>
+      <c r="A38" s="185"/>
       <c r="B38" s="115"/>
       <c r="C38" s="116" t="s">
         <v>108</v>
@@ -6577,221 +6578,221 @@
         <v>628</v>
       </c>
     </row>
-    <row r="39" spans="1:132" s="190" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="136"/>
-      <c r="B39" s="188" t="s">
+    <row r="39" spans="1:132" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="185"/>
+      <c r="B39" s="135" t="s">
         <v>260</v>
       </c>
-      <c r="C39" s="189" t="s">
+      <c r="C39" s="136" t="s">
         <v>259</v>
       </c>
-      <c r="D39" s="190" t="s">
+      <c r="D39" s="137" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="191" t="s">
+      <c r="E39" s="138" t="s">
         <v>643</v>
       </c>
-      <c r="F39" s="191" t="s">
+      <c r="F39" s="138" t="s">
         <v>644</v>
       </c>
-      <c r="G39" s="191" t="s">
+      <c r="G39" s="138" t="s">
         <v>645</v>
       </c>
-      <c r="H39" s="191" t="s">
+      <c r="H39" s="138" t="s">
         <v>646</v>
       </c>
-      <c r="I39" s="191" t="s">
+      <c r="I39" s="138" t="s">
         <v>647</v>
       </c>
-      <c r="J39" s="191" t="s">
+      <c r="J39" s="138" t="s">
         <v>648</v>
       </c>
-      <c r="K39" s="191" t="s">
+      <c r="K39" s="138" t="s">
         <v>455</v>
       </c>
-      <c r="L39" s="191"/>
-      <c r="M39" s="192"/>
-      <c r="N39" s="192"/>
-      <c r="O39" s="193" t="s">
+      <c r="L39" s="138"/>
+      <c r="M39" s="139"/>
+      <c r="N39" s="139"/>
+      <c r="O39" s="140" t="s">
         <v>400</v>
       </c>
-      <c r="P39" s="192" t="s">
+      <c r="P39" s="139" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="40" spans="1:132" s="195" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="136"/>
-      <c r="B40" s="194" t="s">
+    <row r="40" spans="1:132" s="142" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="185"/>
+      <c r="B40" s="141" t="s">
         <v>279</v>
       </c>
-      <c r="C40" s="192" t="s">
+      <c r="C40" s="139" t="s">
         <v>278</v>
       </c>
-      <c r="D40" s="192" t="s">
+      <c r="D40" s="139" t="s">
         <v>159</v>
       </c>
-      <c r="E40" s="192" t="s">
+      <c r="E40" s="139" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="192" t="s">
+      <c r="F40" s="139" t="s">
         <v>181</v>
       </c>
-      <c r="G40" s="192" t="s">
+      <c r="G40" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="H40" s="192" t="s">
+      <c r="H40" s="139" t="s">
         <v>368</v>
       </c>
-      <c r="I40" s="192" t="s">
+      <c r="I40" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="J40" s="192" t="s">
+      <c r="J40" s="139" t="s">
         <v>367</v>
       </c>
-      <c r="K40" s="192" t="s">
+      <c r="K40" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="L40" s="192" t="s">
+      <c r="L40" s="139" t="s">
         <v>167</v>
       </c>
-      <c r="M40" s="192" t="s">
+      <c r="M40" s="139" t="s">
         <v>366</v>
       </c>
-      <c r="N40" s="192" t="s">
+      <c r="N40" s="139" t="s">
         <v>769</v>
       </c>
-      <c r="O40" s="192" t="s">
+      <c r="O40" s="139" t="s">
         <v>167</v>
       </c>
-      <c r="P40" s="192" t="s">
+      <c r="P40" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="Q40" s="192" t="s">
+      <c r="Q40" s="139" t="s">
         <v>213</v>
       </c>
-      <c r="R40" s="192" t="s">
+      <c r="R40" s="139" t="s">
         <v>770</v>
       </c>
-      <c r="S40" s="192"/>
-      <c r="T40" s="192"/>
-      <c r="U40" s="192" t="s">
+      <c r="S40" s="139"/>
+      <c r="T40" s="139"/>
+      <c r="U40" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="V40" s="192" t="s">
+      <c r="V40" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="W40" s="192" t="s">
+      <c r="W40" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="X40" s="192" t="s">
+      <c r="X40" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="Y40" s="192" t="s">
+      <c r="Y40" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="Z40" s="192"/>
-      <c r="AA40" s="192"/>
-      <c r="AB40" s="192"/>
-      <c r="AC40" s="192"/>
-    </row>
-    <row r="41" spans="1:132" s="190" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="136"/>
-      <c r="B41" s="196" t="s">
+      <c r="Z40" s="139"/>
+      <c r="AA40" s="139"/>
+      <c r="AB40" s="139"/>
+      <c r="AC40" s="139"/>
+    </row>
+    <row r="41" spans="1:132" s="137" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="185"/>
+      <c r="B41" s="143" t="s">
         <v>289</v>
       </c>
-      <c r="C41" s="192" t="s">
+      <c r="C41" s="139" t="s">
         <v>288</v>
       </c>
-      <c r="D41" s="192" t="s">
+      <c r="D41" s="139" t="s">
         <v>162</v>
       </c>
-      <c r="E41" s="192" t="s">
+      <c r="E41" s="139" t="s">
         <v>693</v>
       </c>
-      <c r="F41" s="192" t="s">
+      <c r="F41" s="139" t="s">
         <v>694</v>
       </c>
-      <c r="G41" s="192" t="s">
+      <c r="G41" s="139" t="s">
         <v>695</v>
       </c>
-      <c r="H41" s="192" t="s">
+      <c r="H41" s="139" t="s">
         <v>696</v>
       </c>
-      <c r="I41" s="192" t="s">
+      <c r="I41" s="139" t="s">
         <v>697</v>
       </c>
-      <c r="J41" s="192" t="s">
+      <c r="J41" s="139" t="s">
         <v>698</v>
       </c>
-      <c r="K41" s="192" t="s">
+      <c r="K41" s="139" t="s">
         <v>699</v>
       </c>
-      <c r="L41" s="192"/>
-      <c r="M41" s="192"/>
-      <c r="N41" s="192"/>
-      <c r="O41" s="192" t="s">
+      <c r="L41" s="139"/>
+      <c r="M41" s="139"/>
+      <c r="N41" s="139"/>
+      <c r="O41" s="139" t="s">
         <v>700</v>
       </c>
-      <c r="P41" s="192" t="s">
+      <c r="P41" s="139" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="42" spans="1:132" s="198" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="137"/>
-      <c r="B42" s="197" t="s">
+    <row r="42" spans="1:132" s="145" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="186"/>
+      <c r="B42" s="144" t="s">
         <v>267</v>
       </c>
-      <c r="C42" s="192" t="s">
+      <c r="C42" s="139" t="s">
         <v>266</v>
       </c>
-      <c r="D42" s="192" t="s">
+      <c r="D42" s="139" t="s">
         <v>155</v>
       </c>
-      <c r="E42" s="192" t="s">
+      <c r="E42" s="139" t="s">
         <v>372</v>
       </c>
-      <c r="F42" s="192" t="s">
+      <c r="F42" s="139" t="s">
         <v>174</v>
       </c>
-      <c r="G42" s="192" t="s">
+      <c r="G42" s="139" t="s">
         <v>175</v>
       </c>
-      <c r="H42" s="192" t="s">
+      <c r="H42" s="139" t="s">
         <v>176</v>
       </c>
-      <c r="I42" s="192" t="s">
+      <c r="I42" s="139" t="s">
         <v>177</v>
       </c>
-      <c r="J42" s="192"/>
-      <c r="K42" s="192"/>
-      <c r="L42" s="192"/>
-      <c r="M42" s="192"/>
-      <c r="N42" s="192"/>
-      <c r="O42" s="192" t="s">
+      <c r="J42" s="139"/>
+      <c r="K42" s="139"/>
+      <c r="L42" s="139"/>
+      <c r="M42" s="139"/>
+      <c r="N42" s="139"/>
+      <c r="O42" s="139" t="s">
         <v>178</v>
       </c>
-      <c r="P42" s="192" t="s">
+      <c r="P42" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="Q42" s="192"/>
-      <c r="R42" s="192"/>
-      <c r="S42" s="192"/>
-      <c r="T42" s="192"/>
-      <c r="U42" s="192"/>
-      <c r="V42" s="192"/>
-      <c r="W42" s="192"/>
-      <c r="X42" s="192"/>
-      <c r="Y42" s="192"/>
-      <c r="Z42" s="192"/>
-      <c r="AA42" s="192"/>
-      <c r="AB42" s="192"/>
-      <c r="AC42" s="192"/>
+      <c r="Q42" s="139"/>
+      <c r="R42" s="139"/>
+      <c r="S42" s="139"/>
+      <c r="T42" s="139"/>
+      <c r="U42" s="139"/>
+      <c r="V42" s="139"/>
+      <c r="W42" s="139"/>
+      <c r="X42" s="139"/>
+      <c r="Y42" s="139"/>
+      <c r="Z42" s="139"/>
+      <c r="AA42" s="139"/>
+      <c r="AB42" s="139"/>
+      <c r="AC42" s="139"/>
     </row>
     <row r="43" spans="1:132" s="122" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="203" t="s">
+      <c r="A43" s="193" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="204" t="s">
+      <c r="B43" s="150" t="s">
         <v>289</v>
       </c>
       <c r="C43" s="36" t="s">
@@ -6843,12 +6844,12 @@
       <c r="AA43" s="36"/>
       <c r="AB43" s="36"/>
       <c r="AC43" s="36"/>
-      <c r="EA43" s="205"/>
-      <c r="EB43" s="206"/>
+      <c r="EA43" s="151"/>
+      <c r="EB43" s="152"/>
     </row>
     <row r="44" spans="1:132" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="207"/>
-      <c r="B44" s="208" t="s">
+      <c r="A44" s="194"/>
+      <c r="B44" s="153" t="s">
         <v>291</v>
       </c>
       <c r="C44" s="36" t="s">
@@ -6893,12 +6894,12 @@
       <c r="U44" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="EA44" s="209"/>
-      <c r="EB44" s="210"/>
-    </row>
-    <row r="45" spans="1:132" s="212" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="207"/>
-      <c r="B45" s="208" t="s">
+      <c r="EA44" s="154"/>
+      <c r="EB44" s="155"/>
+    </row>
+    <row r="45" spans="1:132" s="157" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="194"/>
+      <c r="B45" s="153" t="s">
         <v>293</v>
       </c>
       <c r="C45" s="36" t="s">
@@ -7051,12 +7052,12 @@
       <c r="DX45" s="36"/>
       <c r="DY45" s="36"/>
       <c r="DZ45" s="36"/>
-      <c r="EA45" s="209"/>
-      <c r="EB45" s="211"/>
-    </row>
-    <row r="46" spans="1:132" s="214" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="207"/>
-      <c r="B46" s="208" t="s">
+      <c r="EA45" s="154"/>
+      <c r="EB45" s="156"/>
+    </row>
+    <row r="46" spans="1:132" s="159" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="194"/>
+      <c r="B46" s="153" t="s">
         <v>295</v>
       </c>
       <c r="C46" s="36" t="s">
@@ -7219,12 +7220,12 @@
       <c r="DX46" s="36"/>
       <c r="DY46" s="36"/>
       <c r="DZ46" s="36"/>
-      <c r="EA46" s="209"/>
-      <c r="EB46" s="213"/>
-    </row>
-    <row r="47" spans="1:132" s="219" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="215"/>
-      <c r="B47" s="216" t="s">
+      <c r="EA46" s="154"/>
+      <c r="EB46" s="158"/>
+    </row>
+    <row r="47" spans="1:132" s="163" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="195"/>
+      <c r="B47" s="160" t="s">
         <v>640</v>
       </c>
       <c r="C47" s="36" t="s">
@@ -7268,168 +7269,168 @@
       <c r="AA47" s="36"/>
       <c r="AB47" s="36"/>
       <c r="AC47" s="36"/>
-      <c r="AD47" s="212"/>
-      <c r="AE47" s="212"/>
-      <c r="AF47" s="212"/>
-      <c r="AG47" s="212"/>
-      <c r="AH47" s="212"/>
-      <c r="AI47" s="212"/>
-      <c r="AJ47" s="212"/>
-      <c r="AK47" s="212"/>
-      <c r="AL47" s="212"/>
-      <c r="AM47" s="212"/>
-      <c r="AN47" s="212"/>
-      <c r="AO47" s="212"/>
-      <c r="AP47" s="212"/>
-      <c r="AQ47" s="212"/>
-      <c r="AR47" s="212"/>
-      <c r="AS47" s="212"/>
-      <c r="AT47" s="212"/>
-      <c r="AU47" s="212"/>
-      <c r="AV47" s="212"/>
-      <c r="AW47" s="212"/>
-      <c r="AX47" s="212"/>
-      <c r="AY47" s="212"/>
-      <c r="AZ47" s="212"/>
-      <c r="BA47" s="212"/>
-      <c r="BB47" s="212"/>
-      <c r="BC47" s="212"/>
-      <c r="BD47" s="212"/>
-      <c r="BE47" s="212"/>
-      <c r="BF47" s="212"/>
-      <c r="BG47" s="212"/>
-      <c r="BH47" s="212"/>
-      <c r="BI47" s="212"/>
-      <c r="BJ47" s="212"/>
-      <c r="BK47" s="212"/>
-      <c r="BL47" s="212"/>
-      <c r="BM47" s="212"/>
-      <c r="BN47" s="212"/>
-      <c r="BO47" s="212"/>
-      <c r="BP47" s="212"/>
-      <c r="BQ47" s="212"/>
-      <c r="BR47" s="212"/>
-      <c r="BS47" s="212"/>
-      <c r="BT47" s="212"/>
-      <c r="BU47" s="212"/>
-      <c r="BV47" s="212"/>
-      <c r="BW47" s="212"/>
-      <c r="BX47" s="212"/>
-      <c r="BY47" s="212"/>
-      <c r="BZ47" s="212"/>
-      <c r="CA47" s="212"/>
-      <c r="CB47" s="212"/>
-      <c r="CC47" s="212"/>
-      <c r="CD47" s="212"/>
-      <c r="CE47" s="212"/>
-      <c r="CF47" s="212"/>
-      <c r="CG47" s="212"/>
-      <c r="CH47" s="212"/>
-      <c r="CI47" s="212"/>
-      <c r="CJ47" s="212"/>
-      <c r="CK47" s="212"/>
-      <c r="CL47" s="212"/>
-      <c r="CM47" s="212"/>
-      <c r="CN47" s="212"/>
-      <c r="CO47" s="212"/>
-      <c r="CP47" s="212"/>
-      <c r="CQ47" s="212"/>
-      <c r="CR47" s="212"/>
-      <c r="CS47" s="212"/>
-      <c r="CT47" s="212"/>
-      <c r="CU47" s="212"/>
-      <c r="CV47" s="212"/>
-      <c r="CW47" s="212"/>
-      <c r="CX47" s="212"/>
-      <c r="CY47" s="212"/>
-      <c r="CZ47" s="212"/>
-      <c r="DA47" s="212"/>
-      <c r="DB47" s="212"/>
-      <c r="DC47" s="212"/>
-      <c r="DD47" s="212"/>
-      <c r="DE47" s="212"/>
-      <c r="DF47" s="212"/>
-      <c r="DG47" s="212"/>
-      <c r="DH47" s="212"/>
-      <c r="DI47" s="212"/>
-      <c r="DJ47" s="212"/>
-      <c r="DK47" s="212"/>
-      <c r="DL47" s="212"/>
-      <c r="DM47" s="212"/>
-      <c r="DN47" s="212"/>
-      <c r="DO47" s="212"/>
-      <c r="DP47" s="212"/>
-      <c r="DQ47" s="212"/>
-      <c r="DR47" s="212"/>
-      <c r="DS47" s="212"/>
-      <c r="DT47" s="212"/>
-      <c r="DU47" s="212"/>
-      <c r="DV47" s="212"/>
-      <c r="DW47" s="212"/>
-      <c r="DX47" s="212"/>
-      <c r="DY47" s="212"/>
-      <c r="DZ47" s="212"/>
-      <c r="EA47" s="217"/>
-      <c r="EB47" s="218"/>
-    </row>
-    <row r="48" spans="1:132" s="221" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="126" t="s">
+      <c r="AD47" s="157"/>
+      <c r="AE47" s="157"/>
+      <c r="AF47" s="157"/>
+      <c r="AG47" s="157"/>
+      <c r="AH47" s="157"/>
+      <c r="AI47" s="157"/>
+      <c r="AJ47" s="157"/>
+      <c r="AK47" s="157"/>
+      <c r="AL47" s="157"/>
+      <c r="AM47" s="157"/>
+      <c r="AN47" s="157"/>
+      <c r="AO47" s="157"/>
+      <c r="AP47" s="157"/>
+      <c r="AQ47" s="157"/>
+      <c r="AR47" s="157"/>
+      <c r="AS47" s="157"/>
+      <c r="AT47" s="157"/>
+      <c r="AU47" s="157"/>
+      <c r="AV47" s="157"/>
+      <c r="AW47" s="157"/>
+      <c r="AX47" s="157"/>
+      <c r="AY47" s="157"/>
+      <c r="AZ47" s="157"/>
+      <c r="BA47" s="157"/>
+      <c r="BB47" s="157"/>
+      <c r="BC47" s="157"/>
+      <c r="BD47" s="157"/>
+      <c r="BE47" s="157"/>
+      <c r="BF47" s="157"/>
+      <c r="BG47" s="157"/>
+      <c r="BH47" s="157"/>
+      <c r="BI47" s="157"/>
+      <c r="BJ47" s="157"/>
+      <c r="BK47" s="157"/>
+      <c r="BL47" s="157"/>
+      <c r="BM47" s="157"/>
+      <c r="BN47" s="157"/>
+      <c r="BO47" s="157"/>
+      <c r="BP47" s="157"/>
+      <c r="BQ47" s="157"/>
+      <c r="BR47" s="157"/>
+      <c r="BS47" s="157"/>
+      <c r="BT47" s="157"/>
+      <c r="BU47" s="157"/>
+      <c r="BV47" s="157"/>
+      <c r="BW47" s="157"/>
+      <c r="BX47" s="157"/>
+      <c r="BY47" s="157"/>
+      <c r="BZ47" s="157"/>
+      <c r="CA47" s="157"/>
+      <c r="CB47" s="157"/>
+      <c r="CC47" s="157"/>
+      <c r="CD47" s="157"/>
+      <c r="CE47" s="157"/>
+      <c r="CF47" s="157"/>
+      <c r="CG47" s="157"/>
+      <c r="CH47" s="157"/>
+      <c r="CI47" s="157"/>
+      <c r="CJ47" s="157"/>
+      <c r="CK47" s="157"/>
+      <c r="CL47" s="157"/>
+      <c r="CM47" s="157"/>
+      <c r="CN47" s="157"/>
+      <c r="CO47" s="157"/>
+      <c r="CP47" s="157"/>
+      <c r="CQ47" s="157"/>
+      <c r="CR47" s="157"/>
+      <c r="CS47" s="157"/>
+      <c r="CT47" s="157"/>
+      <c r="CU47" s="157"/>
+      <c r="CV47" s="157"/>
+      <c r="CW47" s="157"/>
+      <c r="CX47" s="157"/>
+      <c r="CY47" s="157"/>
+      <c r="CZ47" s="157"/>
+      <c r="DA47" s="157"/>
+      <c r="DB47" s="157"/>
+      <c r="DC47" s="157"/>
+      <c r="DD47" s="157"/>
+      <c r="DE47" s="157"/>
+      <c r="DF47" s="157"/>
+      <c r="DG47" s="157"/>
+      <c r="DH47" s="157"/>
+      <c r="DI47" s="157"/>
+      <c r="DJ47" s="157"/>
+      <c r="DK47" s="157"/>
+      <c r="DL47" s="157"/>
+      <c r="DM47" s="157"/>
+      <c r="DN47" s="157"/>
+      <c r="DO47" s="157"/>
+      <c r="DP47" s="157"/>
+      <c r="DQ47" s="157"/>
+      <c r="DR47" s="157"/>
+      <c r="DS47" s="157"/>
+      <c r="DT47" s="157"/>
+      <c r="DU47" s="157"/>
+      <c r="DV47" s="157"/>
+      <c r="DW47" s="157"/>
+      <c r="DX47" s="157"/>
+      <c r="DY47" s="157"/>
+      <c r="DZ47" s="157"/>
+      <c r="EA47" s="161"/>
+      <c r="EB47" s="162"/>
+    </row>
+    <row r="48" spans="1:132" s="165" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="175" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="220" t="s">
+      <c r="B48" s="164" t="s">
         <v>629</v>
       </c>
-      <c r="C48" s="201" t="s">
+      <c r="C48" s="148" t="s">
         <v>110</v>
       </c>
-      <c r="D48" s="200" t="s">
+      <c r="D48" s="147" t="s">
         <v>650</v>
       </c>
-      <c r="E48" s="201" t="s">
+      <c r="E48" s="148" t="s">
         <v>685</v>
       </c>
-      <c r="F48" s="201" t="s">
+      <c r="F48" s="148" t="s">
         <v>686</v>
       </c>
-      <c r="G48" s="201" t="s">
+      <c r="G48" s="148" t="s">
         <v>687</v>
       </c>
-      <c r="H48" s="201" t="s">
+      <c r="H48" s="148" t="s">
         <v>688</v>
       </c>
-      <c r="I48" s="201" t="s">
+      <c r="I48" s="148" t="s">
         <v>689</v>
       </c>
-      <c r="J48" s="201" t="s">
+      <c r="J48" s="148" t="s">
         <v>690</v>
       </c>
-      <c r="K48" s="201"/>
-      <c r="L48" s="201"/>
-      <c r="M48" s="201"/>
-      <c r="N48" s="201"/>
-      <c r="O48" s="201" t="s">
+      <c r="K48" s="148"/>
+      <c r="L48" s="148"/>
+      <c r="M48" s="148"/>
+      <c r="N48" s="148"/>
+      <c r="O48" s="148" t="s">
         <v>691</v>
       </c>
-      <c r="P48" s="201" t="s">
+      <c r="P48" s="148" t="s">
         <v>692</v>
       </c>
-      <c r="Q48" s="201"/>
-      <c r="R48" s="201"/>
-      <c r="S48" s="201"/>
-      <c r="T48" s="201"/>
-      <c r="U48" s="201"/>
-      <c r="V48" s="201"/>
-      <c r="W48" s="201"/>
-      <c r="X48" s="201"/>
-      <c r="Y48" s="201"/>
-      <c r="Z48" s="201"/>
-      <c r="AA48" s="201"/>
-      <c r="AB48" s="201"/>
-      <c r="AC48" s="201"/>
-    </row>
-    <row r="49" spans="1:29" s="202" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="127"/>
-      <c r="B49" s="222" t="s">
+      <c r="Q48" s="148"/>
+      <c r="R48" s="148"/>
+      <c r="S48" s="148"/>
+      <c r="T48" s="148"/>
+      <c r="U48" s="148"/>
+      <c r="V48" s="148"/>
+      <c r="W48" s="148"/>
+      <c r="X48" s="148"/>
+      <c r="Y48" s="148"/>
+      <c r="Z48" s="148"/>
+      <c r="AA48" s="148"/>
+      <c r="AB48" s="148"/>
+      <c r="AC48" s="148"/>
+    </row>
+    <row r="49" spans="1:29" s="149" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="176"/>
+      <c r="B49" s="166" t="s">
         <v>287</v>
       </c>
       <c r="C49" s="35" t="s">
@@ -7475,8 +7476,8 @@
       <c r="AC49" s="35"/>
     </row>
     <row r="50" spans="1:29" s="35" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="127"/>
-      <c r="B50" s="199" t="s">
+      <c r="A50" s="176"/>
+      <c r="B50" s="146" t="s">
         <v>630</v>
       </c>
       <c r="C50" s="35" t="s">
@@ -7514,21 +7515,21 @@
       </c>
     </row>
     <row r="51" spans="1:29" s="85" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="127"/>
+      <c r="A51" s="176"/>
       <c r="B51" s="105"/>
       <c r="C51" s="85" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:29" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="127"/>
+      <c r="A52" s="176"/>
       <c r="B52" s="105"/>
       <c r="C52" s="85" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:29" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="127"/>
+      <c r="A53" s="176"/>
       <c r="B53" s="105"/>
       <c r="C53" s="85" t="s">
         <v>113</v>
@@ -7561,7 +7562,7 @@
       <c r="AC53" s="85"/>
     </row>
     <row r="54" spans="1:29" s="89" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="128"/>
+      <c r="A54" s="177"/>
       <c r="B54" s="106"/>
       <c r="C54" s="85" t="s">
         <v>114</v>
@@ -7594,7 +7595,7 @@
       <c r="AC54" s="85"/>
     </row>
     <row r="55" spans="1:29" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="123" t="s">
+      <c r="A55" s="172" t="s">
         <v>333</v>
       </c>
       <c r="B55" s="121" t="s">
@@ -7679,7 +7680,7 @@
       <c r="AC55" s="36"/>
     </row>
     <row r="56" spans="1:29" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="124"/>
+      <c r="A56" s="173"/>
       <c r="B56" s="108" t="s">
         <v>303</v>
       </c>
@@ -7721,7 +7722,7 @@
       </c>
     </row>
     <row r="57" spans="1:29" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="124"/>
+      <c r="A57" s="173"/>
       <c r="B57" s="108" t="s">
         <v>316</v>
       </c>
@@ -7769,7 +7770,7 @@
       </c>
     </row>
     <row r="58" spans="1:29" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="124"/>
+      <c r="A58" s="173"/>
       <c r="B58" s="108" t="s">
         <v>322</v>
       </c>
@@ -7820,7 +7821,7 @@
       </c>
     </row>
     <row r="59" spans="1:29" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="124"/>
+      <c r="A59" s="173"/>
       <c r="B59" s="108" t="s">
         <v>314</v>
       </c>
@@ -7864,150 +7865,150 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:29" s="224" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="124"/>
-      <c r="B60" s="223" t="s">
+    <row r="60" spans="1:29" s="168" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="173"/>
+      <c r="B60" s="167" t="s">
         <v>318</v>
       </c>
-      <c r="C60" s="224" t="s">
+      <c r="C60" s="168" t="s">
         <v>319</v>
       </c>
-      <c r="D60" s="224" t="s">
+      <c r="D60" s="168" t="s">
         <v>651</v>
       </c>
-      <c r="E60" s="224" t="s">
+      <c r="E60" s="168" t="s">
         <v>733</v>
       </c>
-      <c r="F60" s="224" t="s">
+      <c r="F60" s="168" t="s">
         <v>734</v>
       </c>
-      <c r="G60" s="224" t="s">
+      <c r="G60" s="168" t="s">
         <v>735</v>
       </c>
-      <c r="H60" s="224" t="s">
+      <c r="H60" s="168" t="s">
         <v>736</v>
       </c>
-      <c r="I60" s="224" t="s">
+      <c r="I60" s="168" t="s">
         <v>737</v>
       </c>
-      <c r="J60" s="224" t="s">
+      <c r="J60" s="168" t="s">
         <v>738</v>
       </c>
-      <c r="K60" s="224" t="s">
+      <c r="K60" s="168" t="s">
         <v>740</v>
       </c>
-      <c r="O60" s="224" t="s">
+      <c r="O60" s="168" t="s">
         <v>173</v>
       </c>
-      <c r="P60" s="224" t="s">
+      <c r="P60" s="168" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="61" spans="1:29" s="224" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="124"/>
-      <c r="B61" s="223" t="s">
+    <row r="61" spans="1:29" s="168" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="173"/>
+      <c r="B61" s="167" t="s">
         <v>325</v>
       </c>
-      <c r="C61" s="224" t="s">
+      <c r="C61" s="168" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:29" s="224" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="124"/>
-      <c r="B62" s="223" t="s">
+    <row r="62" spans="1:29" s="168" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="173"/>
+      <c r="B62" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="C62" s="224" t="s">
+      <c r="C62" s="168" t="s">
         <v>328</v>
       </c>
-      <c r="D62" s="224" t="s">
+      <c r="D62" s="168" t="s">
         <v>143</v>
       </c>
-      <c r="E62" s="225" t="s">
+      <c r="E62" s="169" t="s">
         <v>652</v>
       </c>
-      <c r="F62" s="225" t="s">
+      <c r="F62" s="169" t="s">
         <v>653</v>
       </c>
-      <c r="G62" s="225" t="s">
+      <c r="G62" s="169" t="s">
         <v>654</v>
       </c>
-      <c r="H62" s="225" t="s">
+      <c r="H62" s="169" t="s">
         <v>655</v>
       </c>
-      <c r="I62" s="225" t="s">
+      <c r="I62" s="169" t="s">
         <v>656</v>
       </c>
-      <c r="J62" s="225" t="s">
+      <c r="J62" s="169" t="s">
         <v>657</v>
       </c>
-      <c r="K62" s="225" t="s">
+      <c r="K62" s="169" t="s">
         <v>658</v>
       </c>
-      <c r="L62" s="225"/>
-      <c r="O62" s="224" t="s">
+      <c r="L62" s="169"/>
+      <c r="O62" s="168" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="63" spans="1:29" s="224" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="124"/>
-      <c r="B63" s="223" t="s">
+    <row r="63" spans="1:29" s="168" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="173"/>
+      <c r="B63" s="167" t="s">
         <v>329</v>
       </c>
-      <c r="C63" s="224" t="s">
+      <c r="C63" s="168" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="64" spans="1:29" s="227" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="125"/>
-      <c r="B64" s="226" t="s">
+    <row r="64" spans="1:29" s="171" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="174"/>
+      <c r="B64" s="170" t="s">
         <v>331</v>
       </c>
-      <c r="C64" s="224" t="s">
+      <c r="C64" s="168" t="s">
         <v>332</v>
       </c>
-      <c r="D64" s="224" t="s">
+      <c r="D64" s="168" t="s">
         <v>162</v>
       </c>
-      <c r="E64" s="224" t="s">
+      <c r="E64" s="168" t="s">
         <v>711</v>
       </c>
-      <c r="F64" s="224" t="s">
+      <c r="F64" s="168" t="s">
         <v>712</v>
       </c>
-      <c r="G64" s="224" t="s">
+      <c r="G64" s="168" t="s">
         <v>713</v>
       </c>
-      <c r="H64" s="224" t="s">
+      <c r="H64" s="168" t="s">
         <v>714</v>
       </c>
-      <c r="I64" s="224" t="s">
+      <c r="I64" s="168" t="s">
         <v>715</v>
       </c>
-      <c r="J64" s="224" t="s">
+      <c r="J64" s="168" t="s">
         <v>716</v>
       </c>
-      <c r="K64" s="224" t="s">
+      <c r="K64" s="168" t="s">
         <v>717</v>
       </c>
-      <c r="L64" s="224"/>
-      <c r="M64" s="224"/>
-      <c r="N64" s="224"/>
-      <c r="O64" s="224"/>
-      <c r="P64" s="224"/>
-      <c r="Q64" s="224"/>
-      <c r="R64" s="224"/>
-      <c r="S64" s="224"/>
-      <c r="T64" s="224"/>
-      <c r="U64" s="224"/>
-      <c r="V64" s="224"/>
-      <c r="W64" s="224"/>
-      <c r="X64" s="224"/>
-      <c r="Y64" s="224"/>
-      <c r="Z64" s="224"/>
-      <c r="AA64" s="224"/>
-      <c r="AB64" s="224"/>
-      <c r="AC64" s="224"/>
+      <c r="L64" s="168"/>
+      <c r="M64" s="168"/>
+      <c r="N64" s="168"/>
+      <c r="O64" s="168"/>
+      <c r="P64" s="168"/>
+      <c r="Q64" s="168"/>
+      <c r="R64" s="168"/>
+      <c r="S64" s="168"/>
+      <c r="T64" s="168"/>
+      <c r="U64" s="168"/>
+      <c r="V64" s="168"/>
+      <c r="W64" s="168"/>
+      <c r="X64" s="168"/>
+      <c r="Y64" s="168"/>
+      <c r="Z64" s="168"/>
+      <c r="AA64" s="168"/>
+      <c r="AB64" s="168"/>
+      <c r="AC64" s="168"/>
     </row>
     <row r="65" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="79"/>
@@ -8057,13 +8058,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Skillsfuture TSC reference'!$B$2:$B$81</xm:f>
           </x14:formula1>
           <xm:sqref>V3:Z3 U4:Z4 V5:Z64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Skillsfuture TSC reference'!$B$2:$B$81</xm:f>
           </x14:formula1>
@@ -8076,7 +8077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -8102,7 +8103,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="199" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -8110,31 +8111,31 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="148"/>
+      <c r="A3" s="200"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="148"/>
+      <c r="A4" s="200"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="148"/>
+      <c r="A5" s="200"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="148"/>
+      <c r="A6" s="200"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="148"/>
+      <c r="A7" s="200"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8143,19 +8144,19 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="148"/>
+      <c r="A8" s="200"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="149"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="202" t="s">
         <v>81</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -8163,13 +8164,13 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
@@ -8178,91 +8179,91 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="151"/>
+      <c r="A13" s="203"/>
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="151"/>
+      <c r="A14" s="203"/>
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="151"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="151"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="151"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="151"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="151"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="151"/>
+      <c r="A21" s="203"/>
       <c r="B21" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="151"/>
+      <c r="A22" s="203"/>
       <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="151"/>
+      <c r="A23" s="203"/>
       <c r="B23" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="151"/>
+      <c r="A24" s="203"/>
       <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="151"/>
+      <c r="A25" s="203"/>
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="152"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="153" t="s">
+      <c r="A27" s="205" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -8270,91 +8271,91 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="154"/>
+      <c r="A28" s="206"/>
       <c r="B28" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="154"/>
+      <c r="A29" s="206"/>
       <c r="B29" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="154"/>
+      <c r="A30" s="206"/>
       <c r="B30" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="154"/>
+      <c r="A31" s="206"/>
       <c r="B31" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="154"/>
+      <c r="A32" s="206"/>
       <c r="B32" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="154"/>
+      <c r="A33" s="206"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="154"/>
+      <c r="A34" s="206"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="154"/>
+      <c r="A35" s="206"/>
       <c r="B35" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="154"/>
+      <c r="A36" s="206"/>
       <c r="B36" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="154"/>
+      <c r="A37" s="206"/>
       <c r="B37" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="154"/>
+      <c r="A38" s="206"/>
       <c r="B38" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="154"/>
+      <c r="A39" s="206"/>
       <c r="B39" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="154"/>
+      <c r="A40" s="206"/>
       <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="155"/>
+      <c r="A41" s="207"/>
       <c r="B41" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="156" t="s">
+      <c r="A42" s="208" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -8362,13 +8363,13 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="157"/>
+      <c r="A43" s="209"/>
       <c r="B43" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="158" t="s">
+      <c r="A44" s="210" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -8376,73 +8377,73 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="158"/>
+      <c r="A45" s="210"/>
       <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="158"/>
+      <c r="A46" s="210"/>
       <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="158"/>
+      <c r="A47" s="210"/>
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="158"/>
+      <c r="A48" s="210"/>
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="158"/>
+      <c r="A49" s="210"/>
       <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="158"/>
+      <c r="A50" s="210"/>
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="158"/>
+      <c r="A51" s="210"/>
       <c r="B51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="158"/>
+      <c r="A52" s="210"/>
       <c r="B52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="158"/>
+      <c r="A53" s="210"/>
       <c r="B53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="158"/>
+      <c r="A54" s="210"/>
       <c r="B54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="158"/>
+      <c r="A55" s="210"/>
       <c r="B55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="159" t="s">
+      <c r="A56" s="211" t="s">
         <v>85</v>
       </c>
       <c r="B56" s="12" t="s">
@@ -8450,25 +8451,25 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="160"/>
+      <c r="A57" s="212"/>
       <c r="B57" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="160"/>
+      <c r="A58" s="212"/>
       <c r="B58" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="161"/>
+      <c r="A59" s="213"/>
       <c r="B59" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="144" t="s">
+      <c r="A60" s="196" t="s">
         <v>86</v>
       </c>
       <c r="B60" s="14" t="s">
@@ -8476,13 +8477,13 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="145"/>
+      <c r="A61" s="197"/>
       <c r="B61" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="145"/>
+      <c r="A62" s="197"/>
       <c r="B62" s="15" t="s">
         <v>60</v>
       </c>
@@ -8491,7 +8492,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="145"/>
+      <c r="A63" s="197"/>
       <c r="B63" s="15" t="s">
         <v>61</v>
       </c>
@@ -8500,109 +8501,109 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="145"/>
+      <c r="A64" s="197"/>
       <c r="B64" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="145"/>
+      <c r="A65" s="197"/>
       <c r="B65" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="145"/>
+      <c r="A66" s="197"/>
       <c r="B66" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="145"/>
+      <c r="A67" s="197"/>
       <c r="B67" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="145"/>
+      <c r="A68" s="197"/>
       <c r="B68" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="145"/>
+      <c r="A69" s="197"/>
       <c r="B69" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="145"/>
+      <c r="A70" s="197"/>
       <c r="B70" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="145"/>
+      <c r="A71" s="197"/>
       <c r="B71" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="145"/>
+      <c r="A72" s="197"/>
       <c r="B72" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="145"/>
+      <c r="A73" s="197"/>
       <c r="B73" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="145"/>
+      <c r="A74" s="197"/>
       <c r="B74" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="145"/>
+      <c r="A75" s="197"/>
       <c r="B75" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="145"/>
+      <c r="A76" s="197"/>
       <c r="B76" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="145"/>
+      <c r="A77" s="197"/>
       <c r="B77" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="145"/>
+      <c r="A78" s="197"/>
       <c r="B78" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="145"/>
+      <c r="A79" s="197"/>
       <c r="B79" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="145"/>
+      <c r="A80" s="197"/>
       <c r="B80" s="15" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="146"/>
+      <c r="A81" s="198"/>
       <c r="B81" s="16" t="s">
         <v>79</v>
       </c>
@@ -8623,7 +8624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G638"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
@@ -8665,7 +8666,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="217" t="s">
         <v>121</v>
       </c>
       <c r="B2" s="40" t="s">
@@ -8686,7 +8687,7 @@
       <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="165"/>
+      <c r="A3" s="217"/>
       <c r="B3" s="42" t="s">
         <v>306</v>
       </c>
@@ -8705,7 +8706,7 @@
       <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="165"/>
+      <c r="A4" s="217"/>
       <c r="B4" s="40" t="s">
         <v>307</v>
       </c>
@@ -8720,7 +8721,7 @@
       <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="165"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="46" t="s">
         <v>308</v>
       </c>
@@ -8741,7 +8742,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="165"/>
+      <c r="A6" s="217"/>
       <c r="B6" s="40" t="s">
         <v>310</v>
       </c>
@@ -8762,7 +8763,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="165"/>
+      <c r="A7" s="217"/>
       <c r="B7" s="46" t="s">
         <v>320</v>
       </c>
@@ -8781,7 +8782,7 @@
       <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="165"/>
+      <c r="A8" s="217"/>
       <c r="B8" s="40" t="s">
         <v>311</v>
       </c>
@@ -8800,7 +8801,7 @@
       <c r="G8" s="41"/>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="165"/>
+      <c r="A9" s="217"/>
       <c r="B9" s="46" t="s">
         <v>312</v>
       </c>
@@ -8819,7 +8820,7 @@
       <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="165"/>
+      <c r="A10" s="217"/>
       <c r="B10" s="40" t="s">
         <v>313</v>
       </c>
@@ -8838,7 +8839,7 @@
       <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="165"/>
+      <c r="A11" s="217"/>
       <c r="B11" s="46" t="s">
         <v>305</v>
       </c>
@@ -8857,7 +8858,7 @@
       <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="165"/>
+      <c r="A12" s="217"/>
       <c r="B12" s="40" t="s">
         <v>321</v>
       </c>
@@ -8876,7 +8877,7 @@
       <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="218" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="47" t="s">
@@ -8899,7 +8900,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="167"/>
+      <c r="A14" s="219"/>
       <c r="B14" s="48" t="s">
         <v>246</v>
       </c>
@@ -8920,7 +8921,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="167"/>
+      <c r="A15" s="219"/>
       <c r="B15" s="49" t="s">
         <v>248</v>
       </c>
@@ -8941,7 +8942,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="167"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="48" t="s">
         <v>253</v>
       </c>
@@ -8960,7 +8961,7 @@
       <c r="G16" s="41"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="167"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="50" t="s">
         <v>251</v>
       </c>
@@ -8977,7 +8978,7 @@
       <c r="G17" s="41"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="168" t="s">
+      <c r="A18" s="220" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="51" t="s">
@@ -8998,7 +8999,7 @@
       <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
+      <c r="A19" s="215"/>
       <c r="B19" s="52" t="s">
         <v>256</v>
       </c>
@@ -9017,7 +9018,7 @@
       <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
+      <c r="A20" s="215"/>
       <c r="B20" s="48" t="s">
         <v>422</v>
       </c>
@@ -9036,7 +9037,7 @@
       <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="163"/>
+      <c r="A21" s="215"/>
       <c r="B21" s="53" t="s">
         <v>258</v>
       </c>
@@ -9055,7 +9056,7 @@
       <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
+      <c r="A22" s="215"/>
       <c r="B22" s="52" t="s">
         <v>260</v>
       </c>
@@ -9074,7 +9075,7 @@
       <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
+      <c r="A23" s="215"/>
       <c r="B23" s="54" t="s">
         <v>263</v>
       </c>
@@ -9093,7 +9094,7 @@
       <c r="G23" s="41"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
+      <c r="A24" s="215"/>
       <c r="B24" s="52" t="s">
         <v>265</v>
       </c>
@@ -9108,7 +9109,7 @@
       <c r="G24" s="41"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="54" t="s">
         <v>267</v>
       </c>
@@ -9123,7 +9124,7 @@
       <c r="G25" s="41"/>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="221" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="55" t="s">
@@ -9146,7 +9147,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="163"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="54" t="s">
         <v>271</v>
       </c>
@@ -9167,7 +9168,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="163"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="56" t="s">
         <v>273</v>
       </c>
@@ -9188,7 +9189,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="163"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="54" t="s">
         <v>275</v>
       </c>
@@ -9209,7 +9210,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="163"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="56" t="s">
         <v>277</v>
       </c>
@@ -9230,7 +9231,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="163"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="54" t="s">
         <v>279</v>
       </c>
@@ -9251,7 +9252,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="170" t="s">
+      <c r="A32" s="222" t="s">
         <v>118</v>
       </c>
       <c r="B32" s="57" t="s">
@@ -9274,7 +9275,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="170"/>
+      <c r="A33" s="222"/>
       <c r="B33" s="53" t="s">
         <v>285</v>
       </c>
@@ -9293,7 +9294,7 @@
       <c r="G33" s="41"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="171"/>
+      <c r="A34" s="223"/>
       <c r="B34" s="59"/>
       <c r="C34" s="33" t="s">
         <v>108</v>
@@ -9304,7 +9305,7 @@
       <c r="G34" s="41"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="171"/>
+      <c r="A35" s="223"/>
       <c r="B35" s="59" t="s">
         <v>281</v>
       </c>
@@ -9317,7 +9318,7 @@
       <c r="G35" s="41"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="171"/>
+      <c r="A36" s="223"/>
       <c r="B36" s="59"/>
       <c r="C36" s="33" t="s">
         <v>109</v>
@@ -9332,7 +9333,7 @@
       <c r="G36" s="41"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="172" t="s">
+      <c r="A37" s="224" t="s">
         <v>119</v>
       </c>
       <c r="B37" s="51" t="s">
@@ -9353,7 +9354,7 @@
       <c r="G37" s="41"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="173"/>
+      <c r="A38" s="225"/>
       <c r="B38" s="60" t="s">
         <v>291</v>
       </c>
@@ -9372,7 +9373,7 @@
       <c r="G38" s="41"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="173"/>
+      <c r="A39" s="225"/>
       <c r="B39" s="48" t="s">
         <v>293</v>
       </c>
@@ -9391,7 +9392,7 @@
       <c r="G39" s="41"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="173"/>
+      <c r="A40" s="225"/>
       <c r="B40" s="60" t="s">
         <v>295</v>
       </c>
@@ -9410,7 +9411,7 @@
       <c r="G40" s="41"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="162" t="s">
+      <c r="A41" s="214" t="s">
         <v>120</v>
       </c>
       <c r="B41" s="61"/>
@@ -9427,7 +9428,7 @@
       <c r="G41" s="41"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="163"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="62" t="s">
         <v>287</v>
       </c>
@@ -9446,7 +9447,7 @@
       <c r="G42" s="41"/>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="163"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="50"/>
       <c r="C43" s="33" t="s">
         <v>111</v>
@@ -9461,7 +9462,7 @@
       <c r="G43" s="41"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="163"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="50"/>
       <c r="C44" s="33" t="s">
         <v>112</v>
@@ -9478,7 +9479,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="163"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="50"/>
       <c r="C45" s="33" t="s">
         <v>113</v>
@@ -9493,7 +9494,7 @@
       <c r="G45" s="41"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="163"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="50"/>
       <c r="C46" s="33" t="s">
         <v>114</v>
@@ -9508,7 +9509,7 @@
       <c r="G46" s="41"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="164" t="s">
+      <c r="A47" s="216" t="s">
         <v>333</v>
       </c>
       <c r="B47" s="37" t="s">
@@ -9525,7 +9526,7 @@
       <c r="G47" s="41"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="164"/>
+      <c r="A48" s="216"/>
       <c r="B48" s="63" t="s">
         <v>303</v>
       </c>
@@ -9540,7 +9541,7 @@
       <c r="G48" s="41"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="164"/>
+      <c r="A49" s="216"/>
       <c r="B49" s="37" t="s">
         <v>316</v>
       </c>
@@ -9555,7 +9556,7 @@
       <c r="G49" s="41"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="164"/>
+      <c r="A50" s="216"/>
       <c r="B50" s="63" t="s">
         <v>322</v>
       </c>
@@ -9570,7 +9571,7 @@
       <c r="G50" s="41"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="164"/>
+      <c r="A51" s="216"/>
       <c r="B51" s="37" t="s">
         <v>314</v>
       </c>
@@ -9585,7 +9586,7 @@
       <c r="G51" s="41"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="164"/>
+      <c r="A52" s="216"/>
       <c r="B52" s="64" t="s">
         <v>318</v>
       </c>
@@ -9598,7 +9599,7 @@
       <c r="G52" s="41"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="164"/>
+      <c r="A53" s="216"/>
       <c r="B53" s="64" t="s">
         <v>325</v>
       </c>
@@ -9611,7 +9612,7 @@
       <c r="G53" s="41"/>
     </row>
     <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="164"/>
+      <c r="A54" s="216"/>
       <c r="B54" s="64" t="s">
         <v>327</v>
       </c>
@@ -9624,7 +9625,7 @@
       <c r="G54" s="41"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="164"/>
+      <c r="A55" s="216"/>
       <c r="B55" s="64" t="s">
         <v>329</v>
       </c>
@@ -9637,7 +9638,7 @@
       <c r="G55" s="41"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="164"/>
+      <c r="A56" s="216"/>
       <c r="B56" s="64" t="s">
         <v>331</v>
       </c>
@@ -12286,7 +12287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12364,7 +12365,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="226" t="s">
         <v>460</v>
       </c>
       <c r="B2" t="s">
@@ -12423,7 +12424,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="175"/>
+      <c r="A3" s="227"/>
       <c r="B3" t="s">
         <v>300</v>
       </c>
@@ -12441,7 +12442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12496,7 +12497,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="217" t="s">
         <v>121</v>
       </c>
       <c r="B2" s="40" t="s">
@@ -12519,7 +12520,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="165"/>
+      <c r="A3" s="217"/>
       <c r="B3" s="42" t="s">
         <v>306</v>
       </c>
@@ -12552,7 +12553,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="165"/>
+      <c r="A4" s="217"/>
       <c r="B4" s="40" t="s">
         <v>307</v>
       </c>
@@ -12573,7 +12574,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="165"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="69" t="s">
         <v>308</v>
       </c>
@@ -12589,7 +12590,7 @@
       <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="165"/>
+      <c r="A6" s="217"/>
       <c r="B6" s="40" t="s">
         <v>310</v>
       </c>
@@ -12610,7 +12611,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="165"/>
+      <c r="A7" s="217"/>
       <c r="B7" s="66" t="s">
         <v>320</v>
       </c>
@@ -12631,7 +12632,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="165"/>
+      <c r="A8" s="217"/>
       <c r="B8" s="40" t="s">
         <v>311</v>
       </c>
@@ -12664,7 +12665,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="165"/>
+      <c r="A9" s="217"/>
       <c r="B9" s="66" t="s">
         <v>312</v>
       </c>
@@ -12694,7 +12695,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="165"/>
+      <c r="A10" s="217"/>
       <c r="B10" s="40" t="s">
         <v>313</v>
       </c>
@@ -12724,7 +12725,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="165"/>
+      <c r="A11" s="217"/>
       <c r="B11" s="66" t="s">
         <v>305</v>
       </c>
@@ -12733,7 +12734,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="165"/>
+      <c r="A12" s="217"/>
       <c r="B12" s="40" t="s">
         <v>321</v>
       </c>
@@ -12742,7 +12743,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="218" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="67" t="s">
@@ -12765,7 +12766,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="167"/>
+      <c r="A14" s="219"/>
       <c r="B14" s="48" t="s">
         <v>246</v>
       </c>
@@ -12774,7 +12775,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="167"/>
+      <c r="A15" s="219"/>
       <c r="B15" s="49" t="s">
         <v>248</v>
       </c>
@@ -12783,7 +12784,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="167"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="48" t="s">
         <v>253</v>
       </c>
@@ -12792,7 +12793,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="167"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="50" t="s">
         <v>251</v>
       </c>
@@ -12801,7 +12802,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="168" t="s">
+      <c r="A18" s="220" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="51" t="s">
@@ -12812,7 +12813,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
+      <c r="A19" s="215"/>
       <c r="B19" s="52" t="s">
         <v>256</v>
       </c>
@@ -12821,7 +12822,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
+      <c r="A20" s="215"/>
       <c r="B20" s="48" t="s">
         <v>422</v>
       </c>
@@ -12830,7 +12831,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="163"/>
+      <c r="A21" s="215"/>
       <c r="B21" s="53" t="s">
         <v>258</v>
       </c>
@@ -12839,7 +12840,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
+      <c r="A22" s="215"/>
       <c r="B22" s="52" t="s">
         <v>260</v>
       </c>
@@ -12848,7 +12849,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
+      <c r="A23" s="215"/>
       <c r="B23" s="54" t="s">
         <v>263</v>
       </c>
@@ -12857,7 +12858,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
+      <c r="A24" s="215"/>
       <c r="B24" s="52" t="s">
         <v>265</v>
       </c>
@@ -12866,7 +12867,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="54" t="s">
         <v>267</v>
       </c>
@@ -12875,7 +12876,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="169" t="s">
+      <c r="A26" s="221" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="55" t="s">
@@ -12886,7 +12887,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="163"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="54" t="s">
         <v>271</v>
       </c>
@@ -12895,7 +12896,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="163"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="56" t="s">
         <v>273</v>
       </c>
@@ -12904,7 +12905,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="163"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="54" t="s">
         <v>275</v>
       </c>
@@ -12913,7 +12914,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="163"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="56" t="s">
         <v>277</v>
       </c>
@@ -12922,7 +12923,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="163"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="54" t="s">
         <v>279</v>
       </c>
@@ -12931,7 +12932,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="170" t="s">
+      <c r="A32" s="222" t="s">
         <v>118</v>
       </c>
       <c r="B32" s="57" t="s">
@@ -12942,7 +12943,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="170"/>
+      <c r="A33" s="222"/>
       <c r="B33" s="53" t="s">
         <v>285</v>
       </c>
@@ -12951,14 +12952,14 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="171"/>
+      <c r="A34" s="223"/>
       <c r="B34" s="59"/>
       <c r="C34" s="33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="171"/>
+      <c r="A35" s="223"/>
       <c r="B35" s="59" t="s">
         <v>281</v>
       </c>
@@ -12967,14 +12968,14 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="171"/>
+      <c r="A36" s="223"/>
       <c r="B36" s="59"/>
       <c r="C36" s="33" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="172" t="s">
+      <c r="A37" s="224" t="s">
         <v>119</v>
       </c>
       <c r="B37" s="51" t="s">
@@ -12985,7 +12986,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="173"/>
+      <c r="A38" s="225"/>
       <c r="B38" s="60" t="s">
         <v>291</v>
       </c>
@@ -12994,7 +12995,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="173"/>
+      <c r="A39" s="225"/>
       <c r="B39" s="48" t="s">
         <v>293</v>
       </c>
@@ -13003,7 +13004,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="173"/>
+      <c r="A40" s="225"/>
       <c r="B40" s="60" t="s">
         <v>295</v>
       </c>
@@ -13012,7 +13013,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="162" t="s">
+      <c r="A41" s="214" t="s">
         <v>120</v>
       </c>
       <c r="B41" s="61"/>
@@ -13021,7 +13022,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="163"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="62" t="s">
         <v>287</v>
       </c>
@@ -13030,35 +13031,35 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="163"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="50"/>
       <c r="C43" s="33" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="163"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="50"/>
       <c r="C44" s="33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="163"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="50"/>
       <c r="C45" s="33" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="163"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="50"/>
       <c r="C46" s="33" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="164" t="s">
+      <c r="A47" s="216" t="s">
         <v>333</v>
       </c>
       <c r="B47" s="37" t="s">
@@ -13069,7 +13070,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="164"/>
+      <c r="A48" s="216"/>
       <c r="B48" s="63" t="s">
         <v>303</v>
       </c>
@@ -13078,7 +13079,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="164"/>
+      <c r="A49" s="216"/>
       <c r="B49" s="37" t="s">
         <v>316</v>
       </c>
@@ -13087,7 +13088,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="164"/>
+      <c r="A50" s="216"/>
       <c r="B50" s="63" t="s">
         <v>322</v>
       </c>
@@ -13096,7 +13097,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="164"/>
+      <c r="A51" s="216"/>
       <c r="B51" s="37" t="s">
         <v>314</v>
       </c>
@@ -13105,7 +13106,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="164"/>
+      <c r="A52" s="216"/>
       <c r="B52" s="64" t="s">
         <v>318</v>
       </c>
@@ -13114,7 +13115,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="164"/>
+      <c r="A53" s="216"/>
       <c r="B53" s="64" t="s">
         <v>325</v>
       </c>
@@ -13123,7 +13124,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="164"/>
+      <c r="A54" s="216"/>
       <c r="B54" s="64" t="s">
         <v>327</v>
       </c>
@@ -13132,7 +13133,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="164"/>
+      <c r="A55" s="216"/>
       <c r="B55" s="64" t="s">
         <v>329</v>
       </c>
@@ -13141,7 +13142,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="164"/>
+      <c r="A56" s="216"/>
       <c r="B56" s="64" t="s">
         <v>331</v>
       </c>

</xml_diff>